<commit_message>
fixed time formatting and added start and end time to report
</commit_message>
<xml_diff>
--- a/storage/report_excel.xlsx
+++ b/storage/report_excel.xlsx
@@ -357,7 +357,7 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t> 9:12am-17:12pm</t>
+          <t>09:00am-05:30pm</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
@@ -429,7 +429,7 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t> 9:12am-17:12pm</t>
+          <t>09:00am-05:30pm</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
@@ -501,7 +501,7 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t> 9:12am-17:12pm</t>
+          <t>09:00am-05:30pm</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
@@ -557,7 +557,7 @@
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t> 9:12am-17:12pm</t>
+          <t>09:00am-05:30pm</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
@@ -613,7 +613,7 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t> 9:12am-17:12pm</t>
+          <t>09:00am-05:30pm</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">

</xml_diff>